<commit_message>
updating label for question idxxxxx
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
+++ b/WHOVA2016_v1_5_1_XLS_form_for_ODK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="465" windowWidth="11175" windowHeight="7560" activeTab="2"/>
+    <workbookView xWindow="4185" yWindow="465" windowWidth="11175" windowHeight="7560"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -4869,9 +4869,6 @@
     <t xml:space="preserve">(Id10012) </t>
   </si>
   <si>
-    <t>(Id10013) [Did the respondent give consent?]</t>
-  </si>
-  <si>
     <t>(Id10017) What was the first or given name(s) of the deceased?</t>
   </si>
   <si>
@@ -6436,6 +6433,9 @@
   </si>
   <si>
     <t>2016 WHO Verbal Autopsy Form 1.5.1</t>
+  </si>
+  <si>
+    <t>(Id10013) [Did the respondent give consent immediately?]</t>
   </si>
 </sst>
 </file>
@@ -7317,9 +7317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1020"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.6" customHeight="1"/>
@@ -7386,7 +7386,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="90" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="D2" s="38"/>
     </row>
@@ -7534,7 +7534,7 @@
         <v>659</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1566</v>
+        <v>2081</v>
       </c>
       <c r="D13" s="38"/>
       <c r="F13" s="1" t="s">
@@ -7607,7 +7607,7 @@
         <v>660</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="D19" s="38"/>
     </row>
@@ -7619,7 +7619,7 @@
         <v>661</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D20" s="38"/>
     </row>
@@ -7631,7 +7631,7 @@
         <v>662</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="D21" s="38"/>
       <c r="F21" s="1" t="s">
@@ -7646,7 +7646,7 @@
         <v>663</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="D22" s="38"/>
       <c r="F22" s="1" t="s">
@@ -7661,7 +7661,7 @@
         <v>664</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>21</v>
@@ -7681,7 +7681,7 @@
         <v>665</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D24" s="38"/>
       <c r="F24" s="1" t="s">
@@ -7696,7 +7696,7 @@
         <v>1248</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="1" t="s">
@@ -7717,7 +7717,7 @@
         <v>1250</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="1" t="s">
@@ -7735,7 +7735,7 @@
         <v>666</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="D27" s="38"/>
       <c r="I27" s="1" t="s">
@@ -7751,7 +7751,7 @@
         <v>667</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="1" t="s">
@@ -8250,10 +8250,10 @@
         <v>619</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>2075</v>
+      </c>
+      <c r="C56" s="38" t="s">
         <v>2076</v>
-      </c>
-      <c r="C56" s="38" t="s">
-        <v>2077</v>
       </c>
       <c r="D56" s="38"/>
       <c r="E56" s="1" t="s">
@@ -8271,7 +8271,7 @@
         <v>674</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D57" s="38"/>
     </row>
@@ -8288,7 +8288,7 @@
         <v>668</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>74</v>
@@ -8305,7 +8305,7 @@
         <v>669</v>
       </c>
       <c r="C60" s="38" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D60" s="38"/>
       <c r="E60" s="1" t="s">
@@ -8320,7 +8320,7 @@
         <v>670</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>75</v>
@@ -8337,7 +8337,7 @@
         <v>671</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>76</v>
@@ -8354,7 +8354,7 @@
         <v>672</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>1391</v>
@@ -8371,7 +8371,7 @@
         <v>673</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D64" s="38"/>
       <c r="E64" s="1" t="s">
@@ -8386,7 +8386,7 @@
         <v>675</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>77</v>
@@ -8403,7 +8403,7 @@
         <v>1513</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="D66" s="38"/>
       <c r="E66" s="1" t="s">
@@ -8421,7 +8421,7 @@
         <v>676</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D67" s="38"/>
       <c r="E67" s="1" t="s">
@@ -8439,7 +8439,7 @@
         <v>677</v>
       </c>
       <c r="C68" s="38" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="D68" s="38"/>
       <c r="E68" s="1" t="s">
@@ -8454,7 +8454,7 @@
         <v>678</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="D69" s="38"/>
       <c r="E69" s="1" t="s">
@@ -8469,7 +8469,7 @@
         <v>679</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="D70" s="38"/>
       <c r="E70" s="1" t="s">
@@ -8484,7 +8484,7 @@
         <v>680</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="D71" s="38" t="s">
         <v>79</v>
@@ -8501,7 +8501,7 @@
         <v>681</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>80</v>
@@ -8518,7 +8518,7 @@
         <v>682</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="D73" s="38"/>
       <c r="E73" s="1" t="s">
@@ -8552,7 +8552,7 @@
         <v>683</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="D76" s="38"/>
       <c r="F76" s="1" t="s">
@@ -8567,7 +8567,7 @@
         <v>1334</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="D77" s="38"/>
       <c r="E77" s="1" t="s">
@@ -8585,7 +8585,7 @@
         <v>684</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="D78" s="38" t="s">
         <v>75</v>
@@ -8602,7 +8602,7 @@
         <v>1511</v>
       </c>
       <c r="C79" s="38" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="D79" s="38"/>
       <c r="E79" s="1" t="s">
@@ -8620,7 +8620,7 @@
         <v>685</v>
       </c>
       <c r="C80" s="38" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="D80" s="38"/>
       <c r="E80" s="1" t="s">
@@ -8638,7 +8638,7 @@
         <v>686</v>
       </c>
       <c r="C81" s="38" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D81" s="38" t="s">
         <v>75</v>
@@ -8655,7 +8655,7 @@
         <v>687</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="D82" s="38" t="s">
         <v>1392</v>
@@ -8690,7 +8690,7 @@
       </c>
       <c r="D85" s="38"/>
       <c r="E85" s="6" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -8701,7 +8701,7 @@
         <v>710</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="D86" s="38"/>
       <c r="F86" s="1" t="s">
@@ -8716,7 +8716,7 @@
         <v>711</v>
       </c>
       <c r="C87" s="38" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="D87" s="38"/>
       <c r="E87" s="1" t="s">
@@ -8734,7 +8734,7 @@
         <v>712</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="D88" s="38" t="s">
         <v>1171</v>
@@ -8760,7 +8760,7 @@
         <v>713</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="D89" s="38"/>
       <c r="E89" s="1" t="s">
@@ -8778,7 +8778,7 @@
         <v>714</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="D90" s="38" t="s">
         <v>1120</v>
@@ -8804,7 +8804,7 @@
         <v>715</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="D91" s="38"/>
       <c r="F91" s="1" t="s">
@@ -8819,7 +8819,7 @@
         <v>716</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="D92" s="38"/>
       <c r="F92" s="1" t="s">
@@ -8834,7 +8834,7 @@
         <v>717</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="D93" s="38"/>
       <c r="E93" s="1" t="s">
@@ -8852,7 +8852,7 @@
         <v>718</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="D94" s="38"/>
       <c r="E94" s="1" t="s">
@@ -8870,7 +8870,7 @@
         <v>719</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D95" s="38"/>
       <c r="E95" s="1" t="s">
@@ -8888,7 +8888,7 @@
         <v>720</v>
       </c>
       <c r="C96" s="38" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D96" s="38" t="s">
         <v>89</v>
@@ -8908,7 +8908,7 @@
         <v>721</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="D97" s="38"/>
       <c r="F97" s="1" t="s">
@@ -8923,7 +8923,7 @@
         <v>722</v>
       </c>
       <c r="C98" s="38" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="D98" s="38" t="s">
         <v>90</v>
@@ -8962,7 +8962,7 @@
         <v>688</v>
       </c>
       <c r="C101" s="38" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="D101" s="38"/>
       <c r="E101" s="1" t="s">
@@ -8995,7 +8995,7 @@
         <v>689</v>
       </c>
       <c r="C103" s="38" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D103" s="38"/>
       <c r="F103" s="1" t="s">
@@ -9010,7 +9010,7 @@
         <v>690</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="D104" s="38"/>
       <c r="E104" s="1" t="s">
@@ -9028,7 +9028,7 @@
         <v>691</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D105" s="38"/>
       <c r="E105" s="1" t="s">
@@ -9046,7 +9046,7 @@
         <v>1519</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>1096</v>
@@ -9060,7 +9060,7 @@
         <v>692</v>
       </c>
       <c r="C107" s="38" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="D107" s="38" t="s">
         <v>1393</v>
@@ -9080,7 +9080,7 @@
         <v>693</v>
       </c>
       <c r="C108" s="38" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="D108" s="38" t="s">
         <v>1393</v>
@@ -9100,7 +9100,7 @@
         <v>694</v>
       </c>
       <c r="C109" s="38" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="D109" s="38" t="s">
         <v>1393</v>
@@ -9120,7 +9120,7 @@
         <v>695</v>
       </c>
       <c r="C110" s="38" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="D110" s="38" t="s">
         <v>1393</v>
@@ -9140,7 +9140,7 @@
         <v>696</v>
       </c>
       <c r="C111" s="38" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="D111" s="38"/>
       <c r="E111" s="6" t="s">
@@ -9158,7 +9158,7 @@
         <v>697</v>
       </c>
       <c r="C112" s="38" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D112" s="38"/>
       <c r="E112" s="1" t="s">
@@ -9176,7 +9176,7 @@
         <v>698</v>
       </c>
       <c r="C113" s="38" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="D113" s="38"/>
       <c r="E113" s="1" t="s">
@@ -9194,7 +9194,7 @@
         <v>699</v>
       </c>
       <c r="C114" s="38" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D114" s="38" t="s">
         <v>1292</v>
@@ -9214,7 +9214,7 @@
         <v>700</v>
       </c>
       <c r="C115" s="38" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D115" s="38"/>
       <c r="E115" s="1" t="s">
@@ -9232,7 +9232,7 @@
         <v>701</v>
       </c>
       <c r="C116" s="38" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D116" s="38"/>
       <c r="E116" s="1" t="s">
@@ -9250,7 +9250,7 @@
         <v>702</v>
       </c>
       <c r="C117" s="38" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D117" s="38"/>
       <c r="E117" s="1" t="s">
@@ -9268,7 +9268,7 @@
         <v>703</v>
       </c>
       <c r="C118" s="38" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D118" s="38"/>
       <c r="E118" s="1" t="s">
@@ -9286,7 +9286,7 @@
         <v>704</v>
       </c>
       <c r="C119" s="38" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D119" s="38"/>
       <c r="E119" s="1" t="s">
@@ -9304,7 +9304,7 @@
         <v>705</v>
       </c>
       <c r="C120" s="38" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D120" s="38" t="s">
         <v>1393</v>
@@ -9324,7 +9324,7 @@
         <v>706</v>
       </c>
       <c r="C121" s="38" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D121" s="38"/>
       <c r="E121" s="1" t="s">
@@ -9342,7 +9342,7 @@
         <v>707</v>
       </c>
       <c r="C122" s="38" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="D122" s="38"/>
     </row>
@@ -9354,11 +9354,11 @@
         <v>708</v>
       </c>
       <c r="C123" s="38" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="D123" s="38"/>
       <c r="E123" s="1" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="F123" s="1" t="s">
         <v>14</v>
@@ -9372,7 +9372,7 @@
         <v>709</v>
       </c>
       <c r="C124" s="38" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D124" s="38"/>
       <c r="E124" s="1" t="s">
@@ -9416,13 +9416,13 @@
         <v>930</v>
       </c>
       <c r="C128" s="38" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="D128" s="38" t="s">
         <v>1315</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="F128" s="1" t="s">
         <v>14</v>
@@ -9442,7 +9442,7 @@
         <v>979</v>
       </c>
       <c r="C129" s="38" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D129" s="38"/>
       <c r="E129" s="6" t="s">
@@ -9475,7 +9475,7 @@
         <v>1103</v>
       </c>
       <c r="C131" s="38" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D131" s="38" t="s">
         <v>1383</v>
@@ -9501,7 +9501,7 @@
         <v>1105</v>
       </c>
       <c r="C132" s="38" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="D132" s="38"/>
       <c r="E132" s="6" t="s">
@@ -9516,7 +9516,7 @@
         <v>724</v>
       </c>
       <c r="C133" s="38" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="D133" s="38"/>
       <c r="E133" s="6" t="s">
@@ -9540,7 +9540,7 @@
         <v>1044</v>
       </c>
       <c r="C134" s="38" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D134" s="38"/>
       <c r="E134" s="6" t="s">
@@ -9564,7 +9564,7 @@
         <v>1106</v>
       </c>
       <c r="C135" s="38" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="D135" s="38" t="s">
         <v>1107</v>
@@ -9590,7 +9590,7 @@
         <v>723</v>
       </c>
       <c r="C136" s="38" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D136" s="38"/>
       <c r="E136" s="6"/>
@@ -9620,7 +9620,7 @@
         <v>725</v>
       </c>
       <c r="C138" s="38" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D138" s="38" t="s">
         <v>1394</v>
@@ -9655,7 +9655,7 @@
         <v>726</v>
       </c>
       <c r="C140" s="38" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D140" s="38" t="s">
         <v>1395</v>
@@ -9672,7 +9672,7 @@
         <v>727</v>
       </c>
       <c r="C141" s="54" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D141" s="38"/>
       <c r="F141" s="1" t="s">
@@ -9687,7 +9687,7 @@
         <v>728</v>
       </c>
       <c r="C142" s="38" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D142" s="38" t="s">
         <v>1395</v>
@@ -9704,7 +9704,7 @@
         <v>729</v>
       </c>
       <c r="C143" s="38" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D143" s="38" t="s">
         <v>1395</v>
@@ -9721,7 +9721,7 @@
         <v>730</v>
       </c>
       <c r="C144" s="38" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D144" s="38" t="s">
         <v>1395</v>
@@ -9741,7 +9741,7 @@
         <v>731</v>
       </c>
       <c r="C145" s="38" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D145" s="38" t="s">
         <v>1395</v>
@@ -9758,7 +9758,7 @@
         <v>732</v>
       </c>
       <c r="C146" s="38" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D146" s="38" t="s">
         <v>1395</v>
@@ -9775,7 +9775,7 @@
         <v>733</v>
       </c>
       <c r="C147" s="38" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D147" s="38" t="s">
         <v>1395</v>
@@ -9795,7 +9795,7 @@
         <v>734</v>
       </c>
       <c r="C148" s="38" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="D148" s="38" t="s">
         <v>1395</v>
@@ -9812,7 +9812,7 @@
         <v>735</v>
       </c>
       <c r="C149" s="38" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="D149" s="38" t="s">
         <v>1395</v>
@@ -9829,7 +9829,7 @@
         <v>736</v>
       </c>
       <c r="C150" s="38" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="D150" s="38" t="s">
         <v>1395</v>
@@ -9846,7 +9846,7 @@
         <v>737</v>
       </c>
       <c r="C151" s="38" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="D151" s="38" t="s">
         <v>1395</v>
@@ -9863,7 +9863,7 @@
         <v>738</v>
       </c>
       <c r="C152" s="38" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="D152" s="38" t="s">
         <v>1395</v>
@@ -9880,7 +9880,7 @@
         <v>739</v>
       </c>
       <c r="C153" s="38" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D153" s="38" t="s">
         <v>1395</v>
@@ -9900,7 +9900,7 @@
         <v>740</v>
       </c>
       <c r="C154" s="38" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="D154" s="38" t="s">
         <v>1395</v>
@@ -9920,7 +9920,7 @@
         <v>741</v>
       </c>
       <c r="C155" s="38" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="D155" s="38" t="s">
         <v>1395</v>
@@ -9940,7 +9940,7 @@
         <v>742</v>
       </c>
       <c r="C156" s="38" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D156" s="38" t="s">
         <v>1395</v>
@@ -9960,7 +9960,7 @@
         <v>743</v>
       </c>
       <c r="C157" s="38" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="D157" s="38" t="s">
         <v>1395</v>
@@ -9977,7 +9977,7 @@
         <v>744</v>
       </c>
       <c r="C158" s="38" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="D158" s="38" t="s">
         <v>1395</v>
@@ -9994,7 +9994,7 @@
         <v>745</v>
       </c>
       <c r="C159" s="38" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="D159" s="38" t="s">
         <v>1395</v>
@@ -10033,7 +10033,7 @@
         <v>746</v>
       </c>
       <c r="C162" s="38" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="D162" s="38"/>
       <c r="F162" s="1" t="s">
@@ -10048,7 +10048,7 @@
         <v>1181</v>
       </c>
       <c r="C163" s="41" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="D163" s="41" t="s">
         <v>1396</v>
@@ -10074,7 +10074,7 @@
         <v>1187</v>
       </c>
       <c r="C164" s="38" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="D164" s="44" t="s">
         <v>1454</v>
@@ -10095,7 +10095,7 @@
         <v>1182</v>
       </c>
       <c r="C165" s="42" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="D165" s="44" t="s">
         <v>1455</v>
@@ -10121,7 +10121,7 @@
         <v>1188</v>
       </c>
       <c r="C166" s="42" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="D166" s="44" t="s">
         <v>1456</v>
@@ -10147,7 +10147,7 @@
         <v>747</v>
       </c>
       <c r="C167" s="38" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D167" s="38"/>
       <c r="E167" s="1" t="s">
@@ -10165,7 +10165,7 @@
         <v>748</v>
       </c>
       <c r="C168" s="38" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D168" s="38"/>
       <c r="E168" s="1" t="s">
@@ -10183,7 +10183,7 @@
         <v>749</v>
       </c>
       <c r="C169" s="38" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="D169" s="38"/>
       <c r="E169" s="1" t="s">
@@ -10201,7 +10201,7 @@
         <v>750</v>
       </c>
       <c r="C170" s="38" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="D170" s="38"/>
       <c r="E170" s="1" t="s">
@@ -10216,7 +10216,7 @@
         <v>751</v>
       </c>
       <c r="C171" s="38" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D171" s="38"/>
       <c r="E171" s="1" t="s">
@@ -10234,7 +10234,7 @@
         <v>752</v>
       </c>
       <c r="C172" s="38" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D172" s="38"/>
       <c r="F172" s="1" t="s">
@@ -10249,7 +10249,7 @@
         <v>1192</v>
       </c>
       <c r="C173" s="40" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D173" s="44" t="s">
         <v>1454</v>
@@ -10269,7 +10269,7 @@
         <v>1191</v>
       </c>
       <c r="C174" s="40" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D174" s="44" t="s">
         <v>1455</v>
@@ -10295,7 +10295,7 @@
         <v>1194</v>
       </c>
       <c r="C175" s="40" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D175" s="44" t="s">
         <v>1456</v>
@@ -10321,7 +10321,7 @@
         <v>753</v>
       </c>
       <c r="C176" s="38" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="D176" s="38"/>
       <c r="E176" s="1" t="s">
@@ -10339,7 +10339,7 @@
         <v>754</v>
       </c>
       <c r="C177" s="38" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="D177" s="38"/>
       <c r="E177" s="1" t="s">
@@ -10357,7 +10357,7 @@
         <v>755</v>
       </c>
       <c r="C178" s="38" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="D178" s="38"/>
       <c r="E178" s="1" t="s">
@@ -10375,7 +10375,7 @@
         <v>756</v>
       </c>
       <c r="C179" s="38" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="D179" s="38"/>
       <c r="E179" s="1" t="s">
@@ -10393,7 +10393,7 @@
         <v>757</v>
       </c>
       <c r="C180" s="38" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D180" s="38"/>
       <c r="E180" s="1" t="s">
@@ -10411,7 +10411,7 @@
         <v>758</v>
       </c>
       <c r="C181" s="38" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="D181" s="38"/>
       <c r="F181" s="1" t="s">
@@ -10441,7 +10441,7 @@
         <v>1122</v>
       </c>
       <c r="C183" s="38" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D183" s="38" t="s">
         <v>1397</v>
@@ -10467,7 +10467,7 @@
         <v>1123</v>
       </c>
       <c r="C184" s="38" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D184" s="45" t="s">
         <v>1457</v>
@@ -10484,7 +10484,7 @@
         <v>1121</v>
       </c>
       <c r="C185" s="40" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D185" s="44" t="s">
         <v>1455</v>
@@ -10510,7 +10510,7 @@
         <v>760</v>
       </c>
       <c r="C186" s="40" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D186" s="44" t="s">
         <v>1456</v>
@@ -10536,7 +10536,7 @@
         <v>761</v>
       </c>
       <c r="C187" s="40" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D187" s="45" t="s">
         <v>1458</v>
@@ -10562,7 +10562,7 @@
         <v>759</v>
       </c>
       <c r="C188" s="38" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D188" s="38"/>
       <c r="E188" s="6"/>
@@ -10592,7 +10592,7 @@
         <v>762</v>
       </c>
       <c r="C190" s="38" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D190" s="38"/>
       <c r="E190" s="1" t="s">
@@ -10610,7 +10610,7 @@
         <v>763</v>
       </c>
       <c r="C191" s="38" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D191" s="38"/>
       <c r="F191" s="1" t="s">
@@ -10625,7 +10625,7 @@
         <v>1196</v>
       </c>
       <c r="C192" s="41" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D192" s="41" t="s">
         <v>1397</v>
@@ -10651,7 +10651,7 @@
         <v>1197</v>
       </c>
       <c r="C193" s="38" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D193" s="44" t="s">
         <v>1454</v>
@@ -10671,7 +10671,7 @@
         <v>1198</v>
       </c>
       <c r="C194" s="42" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D194" s="44" t="s">
         <v>1455</v>
@@ -10697,7 +10697,7 @@
         <v>1199</v>
       </c>
       <c r="C195" s="42" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D195" s="44" t="s">
         <v>1456</v>
@@ -10723,7 +10723,7 @@
         <v>764</v>
       </c>
       <c r="C196" s="38" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D196" s="38"/>
       <c r="E196" s="1" t="s">
@@ -10741,7 +10741,7 @@
         <v>765</v>
       </c>
       <c r="C197" s="38" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D197" s="38"/>
       <c r="F197" s="1" t="s">
@@ -10756,7 +10756,7 @@
         <v>1204</v>
       </c>
       <c r="C198" s="38" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D198" s="38" t="s">
         <v>1397</v>
@@ -10782,7 +10782,7 @@
         <v>1205</v>
       </c>
       <c r="C199" s="38" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D199" s="44" t="s">
         <v>1454</v>
@@ -10802,7 +10802,7 @@
         <v>1206</v>
       </c>
       <c r="C200" s="42" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="D200" s="44" t="s">
         <v>1455</v>
@@ -10828,7 +10828,7 @@
         <v>1207</v>
       </c>
       <c r="C201" s="42" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D201" s="44" t="s">
         <v>1456</v>
@@ -10854,7 +10854,7 @@
         <v>766</v>
       </c>
       <c r="C202" s="38" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D202" s="38"/>
       <c r="E202" s="1" t="s">
@@ -10872,7 +10872,7 @@
         <v>767</v>
       </c>
       <c r="C203" s="38" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="D203" s="38"/>
       <c r="E203" s="1" t="s">
@@ -10890,7 +10890,7 @@
         <v>768</v>
       </c>
       <c r="C204" s="38" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="D204" s="38"/>
       <c r="E204" s="1" t="s">
@@ -10908,7 +10908,7 @@
         <v>769</v>
       </c>
       <c r="C205" s="38" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D205" s="54" t="s">
         <v>1482</v>
@@ -10928,7 +10928,7 @@
         <v>1339</v>
       </c>
       <c r="C206" s="38" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="D206" s="38"/>
       <c r="E206" s="1" t="s">
@@ -10946,7 +10946,7 @@
         <v>1356</v>
       </c>
       <c r="C207" s="38" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D207" s="38"/>
       <c r="E207" s="1" t="s">
@@ -10964,7 +10964,7 @@
         <v>1340</v>
       </c>
       <c r="C208" s="38" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D208" s="38"/>
       <c r="E208" s="1" t="s">
@@ -10982,7 +10982,7 @@
         <v>770</v>
       </c>
       <c r="C209" s="38" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D209" s="38"/>
       <c r="I209" s="1" t="s">
@@ -10997,7 +10997,7 @@
         <v>771</v>
       </c>
       <c r="C210" s="38" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D210" s="38"/>
       <c r="E210" s="1" t="s">
@@ -11015,7 +11015,7 @@
         <v>772</v>
       </c>
       <c r="C211" s="38" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D211" s="38"/>
       <c r="E211" s="1" t="s">
@@ -11030,7 +11030,7 @@
         <v>773</v>
       </c>
       <c r="C212" s="38" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D212" s="46" t="s">
         <v>1459</v>
@@ -11071,7 +11071,7 @@
         <v>1538</v>
       </c>
       <c r="C214" s="38" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D214" s="46" t="s">
         <v>1543</v>
@@ -11088,7 +11088,7 @@
         <v>774</v>
       </c>
       <c r="C215" s="40" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D215" s="46" t="s">
         <v>1460</v>
@@ -11114,7 +11114,7 @@
         <v>775</v>
       </c>
       <c r="C216" s="40" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D216" s="46" t="s">
         <v>1461</v>
@@ -11140,7 +11140,7 @@
         <v>1134</v>
       </c>
       <c r="C217" s="40" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D217" s="46" t="s">
         <v>1544</v>
@@ -11173,7 +11173,7 @@
         <v>776</v>
       </c>
       <c r="C219" s="38" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D219" s="54" t="s">
         <v>1483</v>
@@ -11190,7 +11190,7 @@
         <v>1212</v>
       </c>
       <c r="C220" s="38" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D220" s="46" t="s">
         <v>1454</v>
@@ -11210,7 +11210,7 @@
         <v>1213</v>
       </c>
       <c r="C221" s="40" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D221" s="44" t="s">
         <v>1455</v>
@@ -11236,7 +11236,7 @@
         <v>1214</v>
       </c>
       <c r="C222" s="40" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D222" s="44" t="s">
         <v>1456</v>
@@ -11262,7 +11262,7 @@
         <v>777</v>
       </c>
       <c r="C223" s="38" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D223" s="38"/>
       <c r="E223" s="18" t="s">
@@ -11280,7 +11280,7 @@
         <v>778</v>
       </c>
       <c r="C224" s="38" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D224" s="38" t="s">
         <v>1161</v>
@@ -11306,7 +11306,7 @@
         <v>1219</v>
       </c>
       <c r="C225" s="38" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D225" s="38" t="s">
         <v>1397</v>
@@ -11332,7 +11332,7 @@
         <v>1220</v>
       </c>
       <c r="C226" s="38" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D226" s="44" t="s">
         <v>1454</v>
@@ -11352,7 +11352,7 @@
         <v>1221</v>
       </c>
       <c r="C227" s="42" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D227" s="44" t="s">
         <v>1455</v>
@@ -11378,7 +11378,7 @@
         <v>1222</v>
       </c>
       <c r="C228" s="42" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D228" s="44" t="s">
         <v>1456</v>
@@ -11404,7 +11404,7 @@
         <v>779</v>
       </c>
       <c r="C229" s="38" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D229" s="38"/>
       <c r="E229" s="1" t="s">
@@ -11422,7 +11422,7 @@
         <v>780</v>
       </c>
       <c r="C230" s="38" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="D230" s="38"/>
       <c r="F230" s="1" t="s">
@@ -11437,7 +11437,7 @@
         <v>781</v>
       </c>
       <c r="C231" s="38" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="D231" s="38"/>
       <c r="E231" s="1" t="s">
@@ -11455,7 +11455,7 @@
         <v>782</v>
       </c>
       <c r="C232" s="38" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D232" s="38"/>
       <c r="F232" s="1" t="s">
@@ -11470,7 +11470,7 @@
         <v>1520</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="F233" s="1" t="s">
         <v>14</v>
@@ -11484,7 +11484,7 @@
         <v>1225</v>
       </c>
       <c r="C234" s="38" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D234" s="44" t="s">
         <v>1454</v>
@@ -11504,7 +11504,7 @@
         <v>1226</v>
       </c>
       <c r="C235" s="40" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D235" s="44" t="s">
         <v>1455</v>
@@ -11530,7 +11530,7 @@
         <v>1227</v>
       </c>
       <c r="C236" s="40" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D236" s="44" t="s">
         <v>1456</v>
@@ -11556,11 +11556,11 @@
         <v>783</v>
       </c>
       <c r="C237" s="38" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D237" s="38"/>
       <c r="E237" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>14</v>
@@ -11574,11 +11574,11 @@
         <v>784</v>
       </c>
       <c r="C238" s="38" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D238" s="38"/>
       <c r="E238" s="1" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="F238" s="1" t="s">
         <v>14</v>
@@ -11592,7 +11592,7 @@
         <v>785</v>
       </c>
       <c r="C239" s="38" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D239" s="38" t="s">
         <v>107</v>
@@ -11612,7 +11612,7 @@
         <v>786</v>
       </c>
       <c r="C240" s="38" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D240" s="38"/>
       <c r="E240" s="1" t="s">
@@ -11630,7 +11630,7 @@
         <v>787</v>
       </c>
       <c r="C241" s="38" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D241" s="38"/>
       <c r="E241" s="1" t="s">
@@ -11661,7 +11661,7 @@
         <v>1137</v>
       </c>
       <c r="C243" s="38" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D243" s="46" t="s">
         <v>1462</v>
@@ -11676,7 +11676,7 @@
         <v>788</v>
       </c>
       <c r="C244" s="40" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D244" s="46" t="s">
         <v>1461</v>
@@ -11702,7 +11702,7 @@
         <v>1142</v>
       </c>
       <c r="C245" s="40" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D245" s="46" t="s">
         <v>1544</v>
@@ -11728,7 +11728,7 @@
         <v>790</v>
       </c>
       <c r="C246" s="40" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D246" s="44" t="s">
         <v>1456</v>
@@ -11743,7 +11743,7 @@
         <v>1160</v>
       </c>
       <c r="L246" s="1" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="247" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11754,7 +11754,7 @@
         <v>789</v>
       </c>
       <c r="C247" s="38" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D247" s="38"/>
       <c r="E247" s="6"/>
@@ -11784,7 +11784,7 @@
         <v>791</v>
       </c>
       <c r="C249" s="38" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D249" s="38"/>
       <c r="E249" s="1" t="s">
@@ -11802,7 +11802,7 @@
         <v>792</v>
       </c>
       <c r="C250" s="38" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D250" s="38"/>
       <c r="E250" s="1" t="s">
@@ -11820,7 +11820,7 @@
         <v>1530</v>
       </c>
       <c r="C251" s="38" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D251" s="44" t="s">
         <v>1454</v>
@@ -11840,7 +11840,7 @@
         <v>1151</v>
       </c>
       <c r="C252" s="40" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D252" s="44" t="s">
         <v>1455</v>
@@ -11866,7 +11866,7 @@
         <v>794</v>
       </c>
       <c r="C253" s="40" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D253" s="44" t="s">
         <v>1456</v>
@@ -11881,7 +11881,7 @@
         <v>1160</v>
       </c>
       <c r="L253" s="1" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="254" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -11892,7 +11892,7 @@
         <v>793</v>
       </c>
       <c r="C254" s="38" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D254" s="38"/>
       <c r="E254" s="1" t="s">
@@ -11917,7 +11917,7 @@
         <v>795</v>
       </c>
       <c r="C255" s="38" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D255" s="38"/>
       <c r="E255" s="1" t="s">
@@ -11935,7 +11935,7 @@
         <v>796</v>
       </c>
       <c r="C256" s="38" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D256" s="38"/>
       <c r="E256" s="1" t="s">
@@ -11953,7 +11953,7 @@
         <v>1534</v>
       </c>
       <c r="C257" s="38" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D257" s="44" t="s">
         <v>1454</v>
@@ -11973,7 +11973,7 @@
         <v>1152</v>
       </c>
       <c r="C258" s="40" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D258" s="44" t="s">
         <v>1455</v>
@@ -11999,7 +11999,7 @@
         <v>798</v>
       </c>
       <c r="C259" s="40" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D259" s="44" t="s">
         <v>1456</v>
@@ -12014,7 +12014,7 @@
         <v>1160</v>
       </c>
       <c r="L259" s="23" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="260" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -12025,7 +12025,7 @@
         <v>797</v>
       </c>
       <c r="C260" s="38" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D260" s="38"/>
       <c r="E260" s="1" t="s">
@@ -12050,7 +12050,7 @@
         <v>799</v>
       </c>
       <c r="C261" s="38" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D261" s="38"/>
       <c r="E261" s="1" t="s">
@@ -12068,7 +12068,7 @@
         <v>800</v>
       </c>
       <c r="C262" s="38" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D262" s="38"/>
       <c r="E262" s="1" t="s">
@@ -12086,7 +12086,7 @@
         <v>1230</v>
       </c>
       <c r="C263" s="38" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D263" s="44" t="s">
         <v>1454</v>
@@ -12106,7 +12106,7 @@
         <v>1231</v>
       </c>
       <c r="C264" s="40" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D264" s="44" t="s">
         <v>1455</v>
@@ -12132,7 +12132,7 @@
         <v>1232</v>
       </c>
       <c r="C265" s="40" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="D265" s="44" t="s">
         <v>1456</v>
@@ -12147,7 +12147,7 @@
         <v>1160</v>
       </c>
       <c r="L265" s="23" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="266" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -12158,7 +12158,7 @@
         <v>801</v>
       </c>
       <c r="C266" s="38" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D266" s="38"/>
       <c r="E266" s="18" t="s">
@@ -12176,7 +12176,7 @@
         <v>802</v>
       </c>
       <c r="C267" s="38" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D267" s="38"/>
       <c r="E267" s="1" t="s">
@@ -12194,7 +12194,7 @@
         <v>1241</v>
       </c>
       <c r="C268" s="38" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D268" s="44" t="s">
         <v>1454</v>
@@ -12214,7 +12214,7 @@
         <v>1242</v>
       </c>
       <c r="C269" s="40" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D269" s="44" t="s">
         <v>1455</v>
@@ -12240,7 +12240,7 @@
         <v>1243</v>
       </c>
       <c r="C270" s="40" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D270" s="44" t="s">
         <v>1456</v>
@@ -12255,7 +12255,7 @@
         <v>1160</v>
       </c>
       <c r="L270" s="23" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="271" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -12266,7 +12266,7 @@
         <v>803</v>
       </c>
       <c r="C271" s="38" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D271" s="38"/>
       <c r="E271" s="18" t="s">
@@ -12284,7 +12284,7 @@
         <v>804</v>
       </c>
       <c r="C272" s="38" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D272" s="38"/>
       <c r="E272" s="1" t="s">
@@ -12302,7 +12302,7 @@
         <v>1253</v>
       </c>
       <c r="C273" s="38" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D273" s="44" t="s">
         <v>1454</v>
@@ -12322,7 +12322,7 @@
         <v>1254</v>
       </c>
       <c r="C274" s="40" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D274" s="44" t="s">
         <v>1455</v>
@@ -12348,7 +12348,7 @@
         <v>1255</v>
       </c>
       <c r="C275" s="40" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D275" s="44" t="s">
         <v>1456</v>
@@ -12363,7 +12363,7 @@
         <v>1160</v>
       </c>
       <c r="L275" s="23" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="276" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -12374,7 +12374,7 @@
         <v>805</v>
       </c>
       <c r="C276" s="38" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D276" s="38"/>
       <c r="E276" s="18" t="s">
@@ -12392,7 +12392,7 @@
         <v>806</v>
       </c>
       <c r="C277" s="38" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D277" s="38"/>
       <c r="F277" s="1" t="s">
@@ -12407,7 +12407,7 @@
         <v>807</v>
       </c>
       <c r="C278" s="38" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D278" s="38"/>
       <c r="E278" s="1" t="s">
@@ -12425,7 +12425,7 @@
         <v>1259</v>
       </c>
       <c r="C279" s="38" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D279" s="44" t="s">
         <v>1463</v>
@@ -12445,7 +12445,7 @@
         <v>1260</v>
       </c>
       <c r="C280" s="40" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D280" s="38" t="s">
         <v>1324</v>
@@ -12471,7 +12471,7 @@
         <v>1261</v>
       </c>
       <c r="C281" s="40" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="D281" s="40" t="s">
         <v>1464</v>
@@ -12497,7 +12497,7 @@
         <v>808</v>
       </c>
       <c r="C282" s="38" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D282" s="38"/>
       <c r="E282" s="1" t="s">
@@ -12515,7 +12515,7 @@
         <v>809</v>
       </c>
       <c r="C283" s="38" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D283" s="38"/>
       <c r="E283" s="1" t="s">
@@ -12533,7 +12533,7 @@
         <v>810</v>
       </c>
       <c r="C284" s="38" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D284" s="38"/>
       <c r="E284" s="1" t="s">
@@ -12551,7 +12551,7 @@
         <v>811</v>
       </c>
       <c r="C285" s="38" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="D285" s="38"/>
       <c r="F285" s="1" t="s">
@@ -12566,7 +12566,7 @@
         <v>812</v>
       </c>
       <c r="C286" s="38" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D286" s="38"/>
       <c r="E286" s="1" t="s">
@@ -12584,7 +12584,7 @@
         <v>813</v>
       </c>
       <c r="C287" s="41" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D287" s="47" t="s">
         <v>1319</v>
@@ -12610,7 +12610,7 @@
         <v>814</v>
       </c>
       <c r="C288" s="38" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D288" s="38"/>
       <c r="E288" s="1" t="s">
@@ -12628,7 +12628,7 @@
         <v>815</v>
       </c>
       <c r="C289" s="38" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D289" s="38" t="s">
         <v>108</v>
@@ -12648,7 +12648,7 @@
         <v>817</v>
       </c>
       <c r="C290" s="38" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="D290" s="38"/>
       <c r="E290" s="1" t="s">
@@ -12666,7 +12666,7 @@
         <v>818</v>
       </c>
       <c r="C291" s="38" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D291" s="38"/>
       <c r="E291" s="1" t="s">
@@ -12684,7 +12684,7 @@
         <v>816</v>
       </c>
       <c r="C292" s="38" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D292" s="38" t="s">
         <v>1398</v>
@@ -12704,7 +12704,7 @@
         <v>819</v>
       </c>
       <c r="C293" s="38" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="D293" s="38"/>
       <c r="E293" s="1" t="s">
@@ -12722,7 +12722,7 @@
         <v>820</v>
       </c>
       <c r="C294" s="38" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="D294" s="38"/>
       <c r="E294" s="1" t="s">
@@ -12740,7 +12740,7 @@
         <v>821</v>
       </c>
       <c r="C295" s="38" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="D295" s="38"/>
       <c r="E295" s="1" t="s">
@@ -12758,7 +12758,7 @@
         <v>822</v>
       </c>
       <c r="C296" s="38" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D296" s="38"/>
       <c r="E296" s="1" t="s">
@@ -12776,7 +12776,7 @@
         <v>823</v>
       </c>
       <c r="C297" s="38" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="D297" s="38"/>
       <c r="E297" s="1" t="s">
@@ -12794,7 +12794,7 @@
         <v>1269</v>
       </c>
       <c r="C298" s="38" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="D298" s="44" t="s">
         <v>1454</v>
@@ -12814,7 +12814,7 @@
         <v>1268</v>
       </c>
       <c r="C299" s="40" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="D299" s="44" t="s">
         <v>1455</v>
@@ -12840,7 +12840,7 @@
         <v>1267</v>
       </c>
       <c r="C300" s="40" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="D300" s="44" t="s">
         <v>1456</v>
@@ -12855,7 +12855,7 @@
         <v>1160</v>
       </c>
       <c r="L300" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="301" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -12866,7 +12866,7 @@
         <v>824</v>
       </c>
       <c r="C301" s="38" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="D301" s="38"/>
       <c r="E301" s="1" t="s">
@@ -12884,7 +12884,7 @@
         <v>825</v>
       </c>
       <c r="C302" s="38" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="D302" s="38"/>
       <c r="F302" s="1" t="s">
@@ -12899,7 +12899,7 @@
         <v>826</v>
       </c>
       <c r="C303" s="38" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D303" s="16" t="s">
         <v>1475</v>
@@ -12925,7 +12925,7 @@
         <v>827</v>
       </c>
       <c r="C304" s="38" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="D304" s="38"/>
       <c r="E304" s="1" t="s">
@@ -12940,14 +12940,14 @@
         <v>619</v>
       </c>
       <c r="B305" s="1" t="s">
+        <v>2072</v>
+      </c>
+      <c r="C305" s="33" t="s">
         <v>2073</v>
-      </c>
-      <c r="C305" s="33" t="s">
-        <v>2074</v>
       </c>
       <c r="D305" s="33"/>
       <c r="E305" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="F305" s="1" t="s">
         <v>14</v>
@@ -12961,7 +12961,7 @@
         <v>828</v>
       </c>
       <c r="C306" s="38" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="D306" s="38"/>
       <c r="E306" s="1" t="s">
@@ -12979,7 +12979,7 @@
         <v>829</v>
       </c>
       <c r="C307" s="38" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D307" s="38"/>
       <c r="E307" s="1" t="s">
@@ -12997,7 +12997,7 @@
         <v>830</v>
       </c>
       <c r="C308" s="38" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D308" s="38"/>
       <c r="E308" s="1" t="s">
@@ -13015,7 +13015,7 @@
         <v>831</v>
       </c>
       <c r="C309" s="38" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D309" s="38"/>
       <c r="E309" s="1" t="s">
@@ -13033,7 +13033,7 @@
         <v>832</v>
       </c>
       <c r="C310" s="38" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D310" s="38"/>
       <c r="E310" s="1" t="s">
@@ -13048,7 +13048,7 @@
         <v>833</v>
       </c>
       <c r="C311" s="38" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D311" s="38"/>
       <c r="F311" s="1" t="s">
@@ -13063,7 +13063,7 @@
         <v>834</v>
       </c>
       <c r="C312" s="38" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D312" s="38"/>
       <c r="E312" s="1" t="s">
@@ -13081,7 +13081,7 @@
         <v>835</v>
       </c>
       <c r="C313" s="38" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D313" s="38"/>
       <c r="E313" s="1" t="s">
@@ -13099,7 +13099,7 @@
         <v>836</v>
       </c>
       <c r="C314" s="38" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D314" s="38"/>
       <c r="E314" s="1" t="s">
@@ -13117,7 +13117,7 @@
         <v>837</v>
       </c>
       <c r="C315" s="38" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D315" s="38"/>
       <c r="E315" s="1" t="s">
@@ -13135,7 +13135,7 @@
         <v>838</v>
       </c>
       <c r="C316" s="38" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D316" s="38"/>
       <c r="E316" s="1" t="s">
@@ -13153,7 +13153,7 @@
         <v>839</v>
       </c>
       <c r="C317" s="38" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D317" s="38"/>
       <c r="E317" s="1" t="s">
@@ -13171,7 +13171,7 @@
         <v>1273</v>
       </c>
       <c r="C318" s="38" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D318" s="44" t="s">
         <v>1454</v>
@@ -13191,7 +13191,7 @@
         <v>1274</v>
       </c>
       <c r="C319" s="40" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D319" s="44" t="s">
         <v>1455</v>
@@ -13217,7 +13217,7 @@
         <v>1275</v>
       </c>
       <c r="C320" s="40" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D320" s="44" t="s">
         <v>1456</v>
@@ -13232,7 +13232,7 @@
         <v>1160</v>
       </c>
       <c r="L320" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="321" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -13243,7 +13243,7 @@
         <v>840</v>
       </c>
       <c r="C321" s="38" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D321" s="38"/>
       <c r="E321" s="1" t="s">
@@ -13261,7 +13261,7 @@
         <v>841</v>
       </c>
       <c r="C322" s="38" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D322" s="38"/>
       <c r="E322" s="1" t="s">
@@ -13279,7 +13279,7 @@
         <v>1280</v>
       </c>
       <c r="C323" s="38" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D323" s="44" t="s">
         <v>1454</v>
@@ -13299,7 +13299,7 @@
         <v>1281</v>
       </c>
       <c r="C324" s="40" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="D324" s="44" t="s">
         <v>1455</v>
@@ -13325,7 +13325,7 @@
         <v>1282</v>
       </c>
       <c r="C325" s="40" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D325" s="44" t="s">
         <v>1456</v>
@@ -13340,7 +13340,7 @@
         <v>1160</v>
       </c>
       <c r="L325" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="326" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -13351,7 +13351,7 @@
         <v>842</v>
       </c>
       <c r="C326" s="38" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D326" s="38"/>
       <c r="E326" s="1" t="s">
@@ -13369,7 +13369,7 @@
         <v>843</v>
       </c>
       <c r="C327" s="38" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="D327" s="38"/>
       <c r="E327" s="1" t="s">
@@ -13387,7 +13387,7 @@
         <v>844</v>
       </c>
       <c r="C328" s="38" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D328" s="38"/>
       <c r="E328" s="1" t="s">
@@ -13405,7 +13405,7 @@
         <v>845</v>
       </c>
       <c r="C329" s="38" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D329" s="38"/>
       <c r="E329" s="1" t="s">
@@ -13423,7 +13423,7 @@
         <v>846</v>
       </c>
       <c r="C330" s="38" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D330" s="38"/>
       <c r="E330" s="1" t="s">
@@ -13441,7 +13441,7 @@
         <v>847</v>
       </c>
       <c r="C331" s="38" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D331" s="38"/>
       <c r="E331" s="1" t="s">
@@ -13459,7 +13459,7 @@
         <v>848</v>
       </c>
       <c r="C332" s="38" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D332" s="38"/>
       <c r="E332" s="1" t="s">
@@ -13477,7 +13477,7 @@
         <v>849</v>
       </c>
       <c r="C333" s="38" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D333" s="38"/>
       <c r="E333" s="1" t="s">
@@ -13495,7 +13495,7 @@
         <v>850</v>
       </c>
       <c r="C334" s="38" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D334" s="38"/>
       <c r="E334" s="1" t="s">
@@ -13513,7 +13513,7 @@
         <v>851</v>
       </c>
       <c r="C335" s="38" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D335" s="38"/>
       <c r="E335" s="1" t="s">
@@ -13531,7 +13531,7 @@
         <v>852</v>
       </c>
       <c r="C336" s="38" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D336" s="38"/>
       <c r="E336" s="1" t="s">
@@ -13549,7 +13549,7 @@
         <v>1484</v>
       </c>
       <c r="C337" s="33" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D337" s="33"/>
       <c r="E337" t="s">
@@ -13567,7 +13567,7 @@
         <v>1556</v>
       </c>
       <c r="C338" s="33" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D338" s="33"/>
       <c r="E338" t="s">
@@ -13585,7 +13585,7 @@
         <v>853</v>
       </c>
       <c r="C339" s="38" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D339" s="38"/>
       <c r="E339" s="1" t="s">
@@ -13603,7 +13603,7 @@
         <v>1288</v>
       </c>
       <c r="C340" s="38" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D340" s="44" t="s">
         <v>1454</v>
@@ -13623,7 +13623,7 @@
         <v>1289</v>
       </c>
       <c r="C341" s="40" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D341" s="44" t="s">
         <v>1455</v>
@@ -13649,7 +13649,7 @@
         <v>1290</v>
       </c>
       <c r="C342" s="40" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D342" s="44" t="s">
         <v>1456</v>
@@ -13664,7 +13664,7 @@
         <v>1160</v>
       </c>
       <c r="L342" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="343" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -13675,7 +13675,7 @@
         <v>854</v>
       </c>
       <c r="C343" s="38" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D343" s="38"/>
       <c r="E343" s="1" t="s">
@@ -13693,7 +13693,7 @@
         <v>855</v>
       </c>
       <c r="C344" s="38" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D344" s="38"/>
       <c r="E344" s="1" t="s">
@@ -13711,7 +13711,7 @@
         <v>856</v>
       </c>
       <c r="C345" s="38" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D345" s="38"/>
       <c r="E345" s="1" t="s">
@@ -13729,7 +13729,7 @@
         <v>857</v>
       </c>
       <c r="C346" s="38" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D346" s="38"/>
       <c r="F346" s="1" t="s">
@@ -13744,7 +13744,7 @@
         <v>1294</v>
       </c>
       <c r="C347" s="38" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D347" s="44" t="s">
         <v>1454</v>
@@ -13764,7 +13764,7 @@
         <v>1295</v>
       </c>
       <c r="C348" s="40" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D348" s="44" t="s">
         <v>1455</v>
@@ -13790,7 +13790,7 @@
         <v>1296</v>
       </c>
       <c r="C349" s="40" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D349" s="44" t="s">
         <v>1456</v>
@@ -13805,7 +13805,7 @@
         <v>1160</v>
       </c>
       <c r="L349" s="23" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="350" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -13816,7 +13816,7 @@
         <v>858</v>
       </c>
       <c r="C350" s="38" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D350" s="38"/>
       <c r="E350" s="1" t="s">
@@ -13834,7 +13834,7 @@
         <v>859</v>
       </c>
       <c r="C351" s="38" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="D351" s="38"/>
       <c r="E351" s="1" t="s">
@@ -13852,7 +13852,7 @@
         <v>860</v>
       </c>
       <c r="C352" s="38" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D352" s="38" t="s">
         <v>109</v>
@@ -13872,7 +13872,7 @@
         <v>861</v>
       </c>
       <c r="C353" s="38" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D353" s="38"/>
       <c r="E353" s="1" t="s">
@@ -13890,7 +13890,7 @@
         <v>862</v>
       </c>
       <c r="C354" s="38" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D354" s="38"/>
       <c r="E354" s="1" t="s">
@@ -13908,7 +13908,7 @@
         <v>863</v>
       </c>
       <c r="C355" s="38" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="D355" s="48" t="s">
         <v>1369</v>
@@ -13925,7 +13925,7 @@
         <v>864</v>
       </c>
       <c r="C356" s="38" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="D356" s="48" t="s">
         <v>1369</v>
@@ -13942,7 +13942,7 @@
         <v>865</v>
       </c>
       <c r="C357" s="38" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D357" s="48" t="s">
         <v>1369</v>
@@ -13962,7 +13962,7 @@
         <v>1304</v>
       </c>
       <c r="C358" s="41" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D358" s="49" t="s">
         <v>1309</v>
@@ -13988,10 +13988,10 @@
         <v>1303</v>
       </c>
       <c r="C359" s="38" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D359" s="44" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="E359" s="18" t="s">
         <v>1310</v>
@@ -14008,7 +14008,7 @@
         <v>1302</v>
       </c>
       <c r="C360" s="42" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="D360" s="44" t="s">
         <v>1455</v>
@@ -14034,7 +14034,7 @@
         <v>1301</v>
       </c>
       <c r="C361" s="42" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="D361" s="44" t="s">
         <v>1551</v>
@@ -14049,7 +14049,7 @@
         <v>1119</v>
       </c>
       <c r="L361" s="23" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="362" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -14060,7 +14060,7 @@
         <v>866</v>
       </c>
       <c r="C362" s="41" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="D362" s="38"/>
       <c r="E362" s="1" t="s">
@@ -14078,7 +14078,7 @@
         <v>867</v>
       </c>
       <c r="C363" s="38" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="D363" s="48" t="s">
         <v>1369</v>
@@ -14098,7 +14098,7 @@
         <v>868</v>
       </c>
       <c r="C364" s="38" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="D364" s="48" t="s">
         <v>1369</v>
@@ -14118,7 +14118,7 @@
         <v>869</v>
       </c>
       <c r="C365" s="38" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="D365" s="48" t="s">
         <v>1369</v>
@@ -14138,7 +14138,7 @@
         <v>870</v>
       </c>
       <c r="C366" s="38" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="D366" s="38" t="s">
         <v>1399</v>
@@ -14158,7 +14158,7 @@
         <v>871</v>
       </c>
       <c r="C367" s="38" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="D367" s="38" t="s">
         <v>1399</v>
@@ -14179,7 +14179,7 @@
         <v>872</v>
       </c>
       <c r="C368" s="38" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="D368" s="50" t="s">
         <v>1369</v>
@@ -14199,7 +14199,7 @@
         <v>873</v>
       </c>
       <c r="C369" s="38" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="D369" s="50" t="s">
         <v>1369</v>
@@ -14219,7 +14219,7 @@
         <v>874</v>
       </c>
       <c r="C370" s="38" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="D370" s="50" t="s">
         <v>1369</v>
@@ -14254,7 +14254,7 @@
         <v>875</v>
       </c>
       <c r="C372" s="38" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="D372" s="38"/>
       <c r="F372" s="1" t="s">
@@ -14269,7 +14269,7 @@
         <v>876</v>
       </c>
       <c r="C373" s="38" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="D373" s="38" t="s">
         <v>1397</v>
@@ -14295,7 +14295,7 @@
         <v>877</v>
       </c>
       <c r="C374" s="38" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="D374" s="38"/>
       <c r="F374" s="1" t="s">
@@ -14310,7 +14310,7 @@
         <v>878</v>
       </c>
       <c r="C375" s="38" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="D375" s="38"/>
       <c r="F375" s="1" t="s">
@@ -14325,7 +14325,7 @@
         <v>879</v>
       </c>
       <c r="C376" s="38" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="D376" s="38"/>
       <c r="F376" s="1" t="s">
@@ -14340,7 +14340,7 @@
         <v>880</v>
       </c>
       <c r="C377" s="38" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="D377" s="38"/>
       <c r="F377" s="1" t="s">
@@ -14355,7 +14355,7 @@
         <v>881</v>
       </c>
       <c r="C378" s="38" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="D378" s="38" t="s">
         <v>1394</v>
@@ -14390,7 +14390,7 @@
       </c>
       <c r="D381" s="38"/>
       <c r="E381" s="6" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="382" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -14401,7 +14401,7 @@
         <v>882</v>
       </c>
       <c r="C382" s="38" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="D382" s="38"/>
       <c r="F382" s="1" t="s">
@@ -14416,7 +14416,7 @@
         <v>883</v>
       </c>
       <c r="C383" s="38" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="D383" s="38"/>
       <c r="F383" s="1" t="s">
@@ -14431,7 +14431,7 @@
         <v>884</v>
       </c>
       <c r="C384" s="38" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="D384" s="38" t="s">
         <v>115</v>
@@ -14448,7 +14448,7 @@
         <v>885</v>
       </c>
       <c r="C385" s="38" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="D385" s="38" t="s">
         <v>116</v>
@@ -14468,7 +14468,7 @@
         <v>886</v>
       </c>
       <c r="C386" s="38" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="D386" s="38"/>
       <c r="E386" s="1" t="s">
@@ -14486,7 +14486,7 @@
         <v>889</v>
       </c>
       <c r="C387" s="38" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="D387" s="38" t="s">
         <v>116</v>
@@ -14506,7 +14506,7 @@
         <v>887</v>
       </c>
       <c r="C388" s="58" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="D388" s="38" t="s">
         <v>117</v>
@@ -14526,7 +14526,7 @@
         <v>890</v>
       </c>
       <c r="C389" s="38" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="D389" s="38"/>
       <c r="E389" s="1" t="s">
@@ -14544,7 +14544,7 @@
         <v>891</v>
       </c>
       <c r="C390" s="41" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="D390" s="47" t="s">
         <v>1320</v>
@@ -14570,7 +14570,7 @@
         <v>888</v>
       </c>
       <c r="C391" s="38" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="D391" s="38" t="s">
         <v>1502</v>
@@ -14590,7 +14590,7 @@
         <v>892</v>
       </c>
       <c r="C392" s="41" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="D392" s="38"/>
       <c r="E392" s="1" t="s">
@@ -14608,7 +14608,7 @@
         <v>893</v>
       </c>
       <c r="C393" s="38" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="D393" s="38"/>
       <c r="E393" s="1" t="s">
@@ -14626,7 +14626,7 @@
         <v>894</v>
       </c>
       <c r="C394" s="38" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="D394" s="38"/>
       <c r="E394" s="1" t="s">
@@ -14644,7 +14644,7 @@
         <v>895</v>
       </c>
       <c r="C395" s="59" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="D395" s="38"/>
       <c r="E395" s="1" t="s">
@@ -14659,7 +14659,7 @@
         <v>896</v>
       </c>
       <c r="C396" s="38" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="D396" s="38"/>
       <c r="E396" s="1" t="s">
@@ -14674,7 +14674,7 @@
         <v>897</v>
       </c>
       <c r="C397" s="38" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="D397" s="38" t="s">
         <v>1311</v>
@@ -14697,7 +14697,7 @@
         <v>898</v>
       </c>
       <c r="C398" s="59" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="D398" s="38" t="s">
         <v>1300</v>
@@ -14717,7 +14717,7 @@
         <v>1516</v>
       </c>
       <c r="C399" s="38" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="D399" s="38"/>
       <c r="E399" s="1" t="s">
@@ -14747,7 +14747,7 @@
         <v>899</v>
       </c>
       <c r="C401" s="38" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="D401" s="38" t="s">
         <v>120</v>
@@ -14764,7 +14764,7 @@
         <v>900</v>
       </c>
       <c r="C402" s="38" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="D402" s="38"/>
       <c r="E402" s="6" t="s">
@@ -14782,7 +14782,7 @@
         <v>901</v>
       </c>
       <c r="C403" s="38" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="D403" s="38"/>
       <c r="E403" s="6" t="s">
@@ -14797,13 +14797,13 @@
         <v>612</v>
       </c>
       <c r="B404" s="1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>1893</v>
+      </c>
+      <c r="E404" s="1" t="s">
         <v>2067</v>
-      </c>
-      <c r="C404" s="1" t="s">
-        <v>1894</v>
-      </c>
-      <c r="E404" s="1" t="s">
-        <v>2068</v>
       </c>
     </row>
     <row r="405" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -14814,13 +14814,13 @@
         <v>1526</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="E405" s="1" t="s">
         <v>1527</v>
       </c>
       <c r="I405" s="1" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="406" spans="1:12" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -14831,7 +14831,7 @@
         <v>902</v>
       </c>
       <c r="C406" s="38" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="D406" s="38" t="s">
         <v>121</v>
@@ -14848,7 +14848,7 @@
         <v>903</v>
       </c>
       <c r="C407" s="38" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="D407" s="38"/>
       <c r="F407" s="1" t="s">
@@ -14863,11 +14863,11 @@
         <v>904</v>
       </c>
       <c r="C408" s="38" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="D408" s="38"/>
       <c r="E408" s="6" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="F408" s="1" t="s">
         <v>14</v>
@@ -14881,7 +14881,7 @@
         <v>905</v>
       </c>
       <c r="C409" s="38" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="D409" s="51" t="s">
         <v>1161</v>
@@ -14904,7 +14904,7 @@
         <v>906</v>
       </c>
       <c r="C410" s="38" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="D410" s="38"/>
       <c r="E410" s="1" t="s">
@@ -14922,7 +14922,7 @@
         <v>907</v>
       </c>
       <c r="C411" s="38" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="D411" s="38"/>
       <c r="F411" s="1" t="s">
@@ -14937,7 +14937,7 @@
         <v>908</v>
       </c>
       <c r="C412" s="38" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="D412" s="38"/>
       <c r="F412" s="1" t="s">
@@ -14952,7 +14952,7 @@
         <v>909</v>
       </c>
       <c r="C413" s="38" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="D413" s="38"/>
       <c r="F413" s="1" t="s">
@@ -14967,7 +14967,7 @@
         <v>910</v>
       </c>
       <c r="C414" s="38" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="D414" s="38"/>
       <c r="F414" s="1" t="s">
@@ -14982,7 +14982,7 @@
         <v>911</v>
       </c>
       <c r="C415" s="40" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="D415" s="38"/>
       <c r="F415" s="1" t="s">
@@ -14997,7 +14997,7 @@
         <v>912</v>
       </c>
       <c r="C416" s="38" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="D416" s="38"/>
       <c r="E416" s="1" t="s">
@@ -15015,7 +15015,7 @@
         <v>913</v>
       </c>
       <c r="C417" s="38" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="D417" s="38" t="s">
         <v>122</v>
@@ -15035,7 +15035,7 @@
         <v>914</v>
       </c>
       <c r="C418" s="38" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="D418" s="38" t="s">
         <v>123</v>
@@ -15052,7 +15052,7 @@
         <v>915</v>
       </c>
       <c r="C419" s="38" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="D419" s="38" t="s">
         <v>124</v>
@@ -15069,7 +15069,7 @@
         <v>916</v>
       </c>
       <c r="C420" s="38" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="D420" s="38"/>
       <c r="F420" s="1" t="s">
@@ -15084,7 +15084,7 @@
         <v>917</v>
       </c>
       <c r="C421" s="38" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="D421" s="38" t="s">
         <v>125</v>
@@ -15101,7 +15101,7 @@
         <v>918</v>
       </c>
       <c r="C422" s="41" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="D422" s="47" t="s">
         <v>1321</v>
@@ -15124,7 +15124,7 @@
         <v>919</v>
       </c>
       <c r="C423" s="38" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="D423" s="38"/>
       <c r="F423" s="1" t="s">
@@ -15139,7 +15139,7 @@
         <v>920</v>
       </c>
       <c r="C424" s="38" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="D424" s="38"/>
       <c r="E424" s="1" t="s">
@@ -15157,7 +15157,7 @@
         <v>921</v>
       </c>
       <c r="C425" s="38" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="D425" s="38"/>
       <c r="E425" s="1" t="s">
@@ -15175,7 +15175,7 @@
         <v>922</v>
       </c>
       <c r="C426" s="38" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D426" s="38"/>
       <c r="E426" s="1" t="s">
@@ -15193,7 +15193,7 @@
         <v>923</v>
       </c>
       <c r="C427" s="38" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="D427" s="38"/>
       <c r="F427" s="1" t="s">
@@ -15208,7 +15208,7 @@
         <v>924</v>
       </c>
       <c r="C428" s="38" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="D428" s="38" t="s">
         <v>1400</v>
@@ -15225,7 +15225,7 @@
         <v>925</v>
       </c>
       <c r="C429" s="38" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="D429" s="38"/>
     </row>
@@ -15237,7 +15237,7 @@
         <v>1067</v>
       </c>
       <c r="C430" s="38" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="D430" s="38"/>
       <c r="F430" s="1" t="s">
@@ -15267,7 +15267,7 @@
         <v>926</v>
       </c>
       <c r="C432" s="38" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="D432" s="38"/>
       <c r="F432" s="1" t="s">
@@ -15282,7 +15282,7 @@
         <v>927</v>
       </c>
       <c r="C433" s="38" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="D433" s="38"/>
       <c r="E433" s="1" t="s">
@@ -15300,7 +15300,7 @@
         <v>928</v>
       </c>
       <c r="C434" s="38" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="D434" s="38"/>
       <c r="E434" s="1" t="s">
@@ -15339,11 +15339,11 @@
         <v>929</v>
       </c>
       <c r="C438" s="38" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="D438" s="38"/>
       <c r="E438" s="1" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="F438" s="1" t="s">
         <v>14</v>
@@ -15369,7 +15369,7 @@
         <v>1360</v>
       </c>
       <c r="C440" s="38" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="D440" s="38" t="s">
         <v>1550</v>
@@ -15389,7 +15389,7 @@
         <v>1362</v>
       </c>
       <c r="C441" s="42" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="D441" s="38" t="s">
         <v>1551</v>
@@ -15415,7 +15415,7 @@
         <v>1363</v>
       </c>
       <c r="C442" s="42" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="D442" s="38" t="s">
         <v>1552</v>
@@ -15441,7 +15441,7 @@
         <v>931</v>
       </c>
       <c r="C443" s="41" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="D443" s="38"/>
       <c r="E443" s="18" t="s">
@@ -15474,7 +15474,7 @@
         <v>932</v>
       </c>
       <c r="C445" s="38" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="D445" s="38" t="s">
         <v>1401</v>
@@ -15494,7 +15494,7 @@
         <v>933</v>
       </c>
       <c r="C446" s="38" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="D446" s="38" t="s">
         <v>1369</v>
@@ -15514,7 +15514,7 @@
         <v>934</v>
       </c>
       <c r="C447" s="38" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="D447" s="38" t="s">
         <v>1402</v>
@@ -15534,7 +15534,7 @@
         <v>935</v>
       </c>
       <c r="C448" s="37" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="D448" s="38" t="s">
         <v>1369</v>
@@ -15569,7 +15569,7 @@
         <v>1435</v>
       </c>
       <c r="C450" s="33" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="D450" s="33" t="s">
         <v>1369</v>
@@ -15587,7 +15587,7 @@
         <v>936</v>
       </c>
       <c r="C451" s="38" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="D451" s="38" t="s">
         <v>1547</v>
@@ -15613,7 +15613,7 @@
         <v>937</v>
       </c>
       <c r="C452" s="38" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="D452" s="38" t="s">
         <v>1545</v>
@@ -15639,7 +15639,7 @@
         <v>1429</v>
       </c>
       <c r="C453" s="33" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="D453" s="33" t="s">
         <v>1546</v>
@@ -15672,7 +15672,7 @@
         <v>938</v>
       </c>
       <c r="C455" s="38" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="D455" s="38" t="s">
         <v>1403</v>
@@ -15692,7 +15692,7 @@
         <v>939</v>
       </c>
       <c r="C456" s="38" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="D456" s="38" t="s">
         <v>1404</v>
@@ -15712,7 +15712,7 @@
         <v>1522</v>
       </c>
       <c r="C457" s="1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="D457" s="1" t="s">
         <v>1523</v>
@@ -15732,7 +15732,7 @@
         <v>940</v>
       </c>
       <c r="C458" s="38" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="D458" s="38" t="s">
         <v>1405</v>
@@ -15752,7 +15752,7 @@
         <v>941</v>
       </c>
       <c r="C459" s="38" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="D459" s="38" t="s">
         <v>1405</v>
@@ -15772,7 +15772,7 @@
         <v>942</v>
       </c>
       <c r="C460" s="38" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="D460" s="38" t="s">
         <v>1405</v>
@@ -15792,7 +15792,7 @@
         <v>1524</v>
       </c>
       <c r="C461" s="33" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="D461" s="33"/>
       <c r="E461" s="1" t="s">
@@ -15810,7 +15810,7 @@
         <v>943</v>
       </c>
       <c r="C462" s="38" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="D462" s="38" t="s">
         <v>1500</v>
@@ -15833,7 +15833,7 @@
         <v>944</v>
       </c>
       <c r="C463" s="38" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="D463" s="38" t="s">
         <v>1161</v>
@@ -15859,7 +15859,7 @@
         <v>945</v>
       </c>
       <c r="C464" s="38" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="D464" s="38"/>
       <c r="E464" s="6" t="s">
@@ -15877,7 +15877,7 @@
         <v>946</v>
       </c>
       <c r="C465" s="38" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="D465" s="38"/>
       <c r="E465" s="6" t="s">
@@ -15895,7 +15895,7 @@
         <v>947</v>
       </c>
       <c r="C466" s="38" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="D466" s="38" t="s">
         <v>1369</v>
@@ -15915,7 +15915,7 @@
         <v>948</v>
       </c>
       <c r="C467" s="38" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="D467" s="38" t="s">
         <v>1369</v>
@@ -15935,7 +15935,7 @@
         <v>949</v>
       </c>
       <c r="C468" s="38" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="D468" s="38" t="s">
         <v>1369</v>
@@ -15955,7 +15955,7 @@
         <v>950</v>
       </c>
       <c r="C469" s="38" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="D469" s="38" t="s">
         <v>1369</v>
@@ -15975,7 +15975,7 @@
         <v>966</v>
       </c>
       <c r="C470" s="38" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="D470" s="38" t="s">
         <v>1161</v>
@@ -16008,7 +16008,7 @@
         <v>134</v>
       </c>
       <c r="C472" s="37" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D472" s="38"/>
       <c r="E472" s="6" t="s">
@@ -16023,7 +16023,7 @@
         <v>951</v>
       </c>
       <c r="C473" s="38" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="D473" s="38"/>
       <c r="F473" s="1" t="s">
@@ -16038,7 +16038,7 @@
         <v>952</v>
       </c>
       <c r="C474" s="38" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="D474" s="38"/>
       <c r="F474" s="1" t="s">
@@ -16068,7 +16068,7 @@
         <v>1153</v>
       </c>
       <c r="C476" s="38" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D476" s="44" t="s">
         <v>1465</v>
@@ -16085,7 +16085,7 @@
         <v>953</v>
       </c>
       <c r="C477" s="40" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D477" s="44" t="s">
         <v>1466</v>
@@ -16111,7 +16111,7 @@
         <v>954</v>
       </c>
       <c r="C478" s="40" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D478" s="44" t="s">
         <v>1467</v>
@@ -16144,7 +16144,7 @@
         <v>955</v>
       </c>
       <c r="C480" s="38" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="D480" s="40" t="s">
         <v>1468</v>
@@ -16164,7 +16164,7 @@
         <v>956</v>
       </c>
       <c r="C481" s="38" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D481" s="38"/>
       <c r="F481" s="1" t="s">
@@ -16179,7 +16179,7 @@
         <v>957</v>
       </c>
       <c r="C482" s="38" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="D482" s="38"/>
       <c r="F482" s="1" t="s">
@@ -16194,7 +16194,7 @@
         <v>958</v>
       </c>
       <c r="C483" s="38" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="D483" s="38"/>
       <c r="F483" s="1" t="s">
@@ -16209,7 +16209,7 @@
         <v>959</v>
       </c>
       <c r="C484" s="37" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="D484" s="38"/>
       <c r="F484" s="6" t="s">
@@ -16224,7 +16224,7 @@
         <v>960</v>
       </c>
       <c r="C485" s="38" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="D485" s="38"/>
       <c r="F485" s="1" t="s">
@@ -16239,7 +16239,7 @@
         <v>961</v>
       </c>
       <c r="C486" s="38" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D486" s="38"/>
       <c r="E486" s="1" t="s">
@@ -16257,7 +16257,7 @@
         <v>962</v>
       </c>
       <c r="C487" s="38" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="D487" s="38"/>
       <c r="E487" s="1" t="s">
@@ -16275,7 +16275,7 @@
         <v>1372</v>
       </c>
       <c r="C488" s="38" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D488" s="38"/>
       <c r="E488" s="1" t="s">
@@ -16300,7 +16300,7 @@
         <v>963</v>
       </c>
       <c r="C490" s="38" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="D490" s="38"/>
       <c r="F490" s="1" t="s">
@@ -16315,7 +16315,7 @@
         <v>964</v>
       </c>
       <c r="C491" s="38" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="D491" s="38" t="s">
         <v>1161</v>
@@ -16341,7 +16341,7 @@
         <v>965</v>
       </c>
       <c r="C492" s="38" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="D492" s="38"/>
       <c r="E492" s="1" t="s">
@@ -16361,7 +16361,7 @@
         <v>967</v>
       </c>
       <c r="C493" s="38" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="D493" s="38"/>
     </row>
@@ -16373,7 +16373,7 @@
         <v>968</v>
       </c>
       <c r="C494" s="38" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="D494" s="38"/>
       <c r="F494" s="1" t="s">
@@ -16388,7 +16388,7 @@
         <v>969</v>
       </c>
       <c r="C495" s="38" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="D495" s="38"/>
     </row>
@@ -16400,7 +16400,7 @@
         <v>970</v>
       </c>
       <c r="C496" s="38" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="D496" s="38"/>
       <c r="F496" s="1" t="s">
@@ -16415,7 +16415,7 @@
         <v>971</v>
       </c>
       <c r="C497" s="38" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="D497" s="38"/>
       <c r="F497" s="1" t="s">
@@ -16430,7 +16430,7 @@
         <v>972</v>
       </c>
       <c r="C498" s="38" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="D498" s="38"/>
       <c r="F498" s="1" t="s">
@@ -16445,7 +16445,7 @@
         <v>973</v>
       </c>
       <c r="C499" s="38" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="D499" s="38"/>
     </row>
@@ -16457,7 +16457,7 @@
         <v>974</v>
       </c>
       <c r="C500" s="38" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="D500" s="38"/>
       <c r="F500" s="1" t="s">
@@ -16472,7 +16472,7 @@
         <v>975</v>
       </c>
       <c r="C501" s="38" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="D501" s="38"/>
       <c r="F501" s="1" t="s">
@@ -16487,7 +16487,7 @@
         <v>976</v>
       </c>
       <c r="C502" s="38" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="D502" s="38"/>
       <c r="F502" s="1" t="s">
@@ -16502,7 +16502,7 @@
         <v>977</v>
       </c>
       <c r="C503" s="41" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="D503" s="41"/>
       <c r="F503" s="18" t="s">
@@ -16517,7 +16517,7 @@
         <v>978</v>
       </c>
       <c r="C504" s="38" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="D504" s="38"/>
       <c r="F504" s="1" t="s">
@@ -16561,7 +16561,7 @@
         <v>980</v>
       </c>
       <c r="C508" s="38" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="D508" s="38"/>
       <c r="F508" s="1" t="s">
@@ -16576,7 +16576,7 @@
         <v>1528</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="F509" s="1" t="s">
         <v>14</v>
@@ -16590,7 +16590,7 @@
         <v>981</v>
       </c>
       <c r="C510" s="38" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="D510" s="38"/>
       <c r="F510" s="1" t="s">
@@ -16605,11 +16605,11 @@
         <v>982</v>
       </c>
       <c r="C511" s="38" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D511" s="38"/>
       <c r="E511" s="1" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="F511" s="1" t="s">
         <v>14</v>
@@ -16620,14 +16620,14 @@
         <v>619</v>
       </c>
       <c r="B512" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="C512" s="38" t="s">
         <v>2064</v>
-      </c>
-      <c r="C512" s="38" t="s">
-        <v>2065</v>
       </c>
       <c r="D512" s="38"/>
       <c r="E512" s="1" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="F512" s="1" t="s">
         <v>14</v>
@@ -16641,7 +16641,7 @@
         <v>983</v>
       </c>
       <c r="C513" s="38" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="D513" s="38" t="s">
         <v>1161</v>
@@ -16667,7 +16667,7 @@
         <v>1101</v>
       </c>
       <c r="C514" s="38" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="D514" s="38" t="s">
         <v>1161</v>
@@ -16715,7 +16715,7 @@
         <v>984</v>
       </c>
       <c r="C517" s="38" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="D517" s="38"/>
       <c r="F517" s="1" t="s">
@@ -16730,7 +16730,7 @@
         <v>985</v>
       </c>
       <c r="C518" s="38" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="D518" s="38"/>
       <c r="E518" s="1" t="s">
@@ -16748,7 +16748,7 @@
         <v>986</v>
       </c>
       <c r="C519" s="38" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="D519" s="38"/>
       <c r="E519" s="1" t="s">
@@ -16766,7 +16766,7 @@
         <v>987</v>
       </c>
       <c r="C520" s="38" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="D520" s="38"/>
       <c r="E520" s="1" t="s">
@@ -16784,7 +16784,7 @@
         <v>988</v>
       </c>
       <c r="C521" s="38" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="D521" s="38"/>
       <c r="E521" s="1" t="s">
@@ -16802,7 +16802,7 @@
         <v>989</v>
       </c>
       <c r="C522" s="38" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="D522" s="38"/>
       <c r="E522" s="1" t="s">
@@ -16820,7 +16820,7 @@
         <v>990</v>
       </c>
       <c r="C523" s="38" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="D523" s="38"/>
       <c r="E523" s="1" t="s">
@@ -16838,7 +16838,7 @@
         <v>991</v>
       </c>
       <c r="C524" s="38" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D524" s="38"/>
       <c r="E524" s="1" t="s">
@@ -16856,7 +16856,7 @@
         <v>992</v>
       </c>
       <c r="C525" s="38" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="D525" s="38"/>
       <c r="E525" s="1" t="s">
@@ -16874,7 +16874,7 @@
         <v>993</v>
       </c>
       <c r="C526" s="38" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="D526" s="38"/>
       <c r="E526" s="1" t="s">
@@ -16892,7 +16892,7 @@
         <v>994</v>
       </c>
       <c r="C527" s="40" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="D527" s="38"/>
       <c r="E527" s="1" t="s">
@@ -16910,7 +16910,7 @@
         <v>995</v>
       </c>
       <c r="C528" s="38" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D528" s="38" t="s">
         <v>1374</v>
@@ -16930,7 +16930,7 @@
         <v>996</v>
       </c>
       <c r="C529" s="38" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D529" s="38" t="s">
         <v>142</v>
@@ -16950,7 +16950,7 @@
         <v>997</v>
       </c>
       <c r="C530" s="33" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="D530" s="33"/>
       <c r="E530" s="1" t="s">
@@ -16965,7 +16965,7 @@
         <v>1414</v>
       </c>
       <c r="C531" s="33" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="D531" s="33"/>
       <c r="E531" s="1" t="s">
@@ -16983,7 +16983,7 @@
         <v>998</v>
       </c>
       <c r="C532" s="38" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="D532" s="38"/>
       <c r="F532" s="1" t="s">
@@ -16998,7 +16998,7 @@
         <v>999</v>
       </c>
       <c r="C533" s="38" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="D533" s="38"/>
       <c r="E533" s="1" t="s">
@@ -17016,7 +17016,7 @@
         <v>1332</v>
       </c>
       <c r="C534" s="38" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="D534" s="38"/>
       <c r="E534" s="1" t="s">
@@ -17034,7 +17034,7 @@
         <v>1000</v>
       </c>
       <c r="C535" s="38" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D535" s="38"/>
       <c r="E535" s="1" t="s">
@@ -17052,7 +17052,7 @@
         <v>1001</v>
       </c>
       <c r="C536" s="38" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="D536" s="38"/>
       <c r="F536" s="1" t="s">
@@ -17067,7 +17067,7 @@
         <v>1002</v>
       </c>
       <c r="C537" s="38" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D537" s="38"/>
       <c r="E537" s="1" t="s">
@@ -17085,7 +17085,7 @@
         <v>1003</v>
       </c>
       <c r="C538" s="38" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D538" s="38"/>
       <c r="E538" s="1" t="s">
@@ -17103,7 +17103,7 @@
         <v>1004</v>
       </c>
       <c r="C539" s="38" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D539" s="38"/>
       <c r="E539" s="1" t="s">
@@ -17121,7 +17121,7 @@
         <v>1504</v>
       </c>
       <c r="C540" s="38" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="D540" s="38"/>
       <c r="E540" s="1" t="s">
@@ -17139,7 +17139,7 @@
         <v>1005</v>
       </c>
       <c r="C541" s="38" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D541" s="38"/>
       <c r="E541" s="1" t="s">
@@ -17157,7 +17157,7 @@
         <v>1506</v>
       </c>
       <c r="C542" s="38" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D542" s="38"/>
       <c r="E542" s="1" t="s">
@@ -17175,7 +17175,7 @@
         <v>1006</v>
       </c>
       <c r="C543" s="38" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D543" s="38"/>
       <c r="E543" s="1" t="s">
@@ -17193,7 +17193,7 @@
         <v>1508</v>
       </c>
       <c r="C544" s="38" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D544" s="38"/>
       <c r="E544" s="1" t="s">
@@ -17211,7 +17211,7 @@
         <v>1007</v>
       </c>
       <c r="C545" s="38" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D545" s="38"/>
       <c r="E545" s="1" t="s">
@@ -17229,7 +17229,7 @@
         <v>1008</v>
       </c>
       <c r="C546" s="38" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D546" s="38" t="s">
         <v>143</v>
@@ -17249,7 +17249,7 @@
         <v>1009</v>
       </c>
       <c r="C547" s="38" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D547" s="38"/>
       <c r="E547" s="1" t="s">
@@ -17267,7 +17267,7 @@
         <v>1010</v>
       </c>
       <c r="C548" s="38" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D548" s="38"/>
       <c r="E548" s="1" t="s">
@@ -17285,7 +17285,7 @@
         <v>1011</v>
       </c>
       <c r="C549" s="38" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D549" s="38"/>
       <c r="E549" s="1" t="s">
@@ -17303,7 +17303,7 @@
         <v>1012</v>
       </c>
       <c r="C550" s="38" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D550" s="38"/>
       <c r="E550" s="1" t="s">
@@ -17347,7 +17347,7 @@
         <v>1013</v>
       </c>
       <c r="C554" s="38" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D554" s="38" t="s">
         <v>1378</v>
@@ -17364,7 +17364,7 @@
         <v>1014</v>
       </c>
       <c r="C555" s="38" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="D555" s="52" t="s">
         <v>1469</v>
@@ -17384,7 +17384,7 @@
         <v>1015</v>
       </c>
       <c r="C556" s="38" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="D556" s="52" t="s">
         <v>1469</v>
@@ -17404,7 +17404,7 @@
         <v>1016</v>
       </c>
       <c r="C557" s="38" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="D557" s="52" t="s">
         <v>1469</v>
@@ -17424,7 +17424,7 @@
         <v>1017</v>
       </c>
       <c r="C558" s="38" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="D558" s="52" t="s">
         <v>1470</v>
@@ -17444,7 +17444,7 @@
         <v>1018</v>
       </c>
       <c r="C559" s="38" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="D559" s="52" t="s">
         <v>1471</v>
@@ -17461,7 +17461,7 @@
         <v>1019</v>
       </c>
       <c r="C560" s="38" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="D560" s="52" t="s">
         <v>1472</v>
@@ -17478,7 +17478,7 @@
         <v>1020</v>
       </c>
       <c r="C561" s="38" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="D561" s="52" t="s">
         <v>1472</v>
@@ -17495,7 +17495,7 @@
         <v>1021</v>
       </c>
       <c r="C562" s="38" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="D562" s="52"/>
       <c r="F562" s="1" t="s">
@@ -17510,7 +17510,7 @@
         <v>1022</v>
       </c>
       <c r="C563" s="38" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="D563" s="52"/>
       <c r="F563" s="1" t="s">
@@ -17544,7 +17544,7 @@
         <v>1023</v>
       </c>
       <c r="C566" s="38" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="D566" s="38" t="s">
         <v>1406</v>
@@ -17561,7 +17561,7 @@
         <v>1024</v>
       </c>
       <c r="C567" s="38" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="D567" s="38" t="s">
         <v>1407</v>
@@ -17581,7 +17581,7 @@
         <v>1025</v>
       </c>
       <c r="C568" s="38" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="D568" s="38"/>
       <c r="E568" s="1" t="s">
@@ -17599,7 +17599,7 @@
         <v>1026</v>
       </c>
       <c r="C569" s="38" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="D569" s="38" t="s">
         <v>149</v>
@@ -17616,7 +17616,7 @@
         <v>1027</v>
       </c>
       <c r="C570" s="38" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="D570" s="38" t="s">
         <v>148</v>
@@ -17633,7 +17633,7 @@
         <v>1028</v>
       </c>
       <c r="C571" s="38" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="D571" s="38"/>
       <c r="E571" s="1" t="s">
@@ -17648,7 +17648,7 @@
         <v>1029</v>
       </c>
       <c r="C572" s="38" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="D572" s="38"/>
       <c r="E572" s="1" t="s">
@@ -17663,7 +17663,7 @@
         <v>1030</v>
       </c>
       <c r="C573" s="38" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="D573" s="38"/>
       <c r="E573" s="1" t="s">
@@ -17678,7 +17678,7 @@
         <v>1031</v>
       </c>
       <c r="C574" s="38" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="D574" s="38"/>
       <c r="E574" s="1" t="s">
@@ -17693,7 +17693,7 @@
         <v>1032</v>
       </c>
       <c r="C575" s="38" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="D575" s="38"/>
       <c r="E575" s="1" t="s">
@@ -17708,7 +17708,7 @@
         <v>1033</v>
       </c>
       <c r="C576" s="38" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="D576" s="38"/>
       <c r="E576" s="1" t="s">
@@ -17723,7 +17723,7 @@
         <v>1034</v>
       </c>
       <c r="C577" s="38" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="D577" s="38"/>
       <c r="E577" s="1" t="s">
@@ -17760,7 +17760,7 @@
         <v>1035</v>
       </c>
       <c r="C580" s="38" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="D580" s="38" t="s">
         <v>1408</v>
@@ -17777,7 +17777,7 @@
         <v>1036</v>
       </c>
       <c r="C581" s="38" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="D581" s="38"/>
       <c r="E581" s="1" t="s">
@@ -17792,7 +17792,7 @@
         <v>1037</v>
       </c>
       <c r="C582" s="38" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="D582" s="38"/>
       <c r="E582" s="1" t="s">
@@ -17807,7 +17807,7 @@
         <v>1038</v>
       </c>
       <c r="C583" s="38" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="D583" s="38"/>
       <c r="E583" s="1" t="s">
@@ -17829,7 +17829,7 @@
         <v>1354</v>
       </c>
       <c r="C585" s="38" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="D585" s="38"/>
       <c r="E585" s="1" t="s">
@@ -17847,7 +17847,7 @@
         <v>1355</v>
       </c>
       <c r="C586" s="38" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="D586" s="38"/>
       <c r="E586" s="1" t="s">
@@ -17865,7 +17865,7 @@
         <v>1353</v>
       </c>
       <c r="C587" s="38" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="D587" s="38"/>
       <c r="E587" s="1" t="s">
@@ -17895,7 +17895,7 @@
         <v>1481</v>
       </c>
       <c r="C589" s="38" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D589" s="38"/>
     </row>
@@ -20687,10 +20687,10 @@
         <v>1293</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -23649,7 +23649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -23680,13 +23680,13 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B2" s="27">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="D2" t="s">
         <v>514</v>

</xml_diff>